<commit_message>
Drafting poster, updated surgery info with estimatesx
</commit_message>
<xml_diff>
--- a/AUGpostop/studydata/AUG_surgery.xlsx
+++ b/AUGpostop/studydata/AUG_surgery.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24150" windowHeight="12960" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="AugmentedPhysiologic_DATA_LABEL" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Tiffany</author>
+  </authors>
+  <commentList>
+    <comment ref="W16" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Tiffany:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Estimated</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="73">
   <si>
     <t>Study ID</t>
   </si>
@@ -229,26 +263,54 @@
   </si>
   <si>
     <t>Aortic Arch Hypoplasia and Coarctation</t>
+  </si>
+  <si>
+    <t>AUG100</t>
+  </si>
+  <si>
+    <t>AUG101</t>
+  </si>
+  <si>
+    <t>AUG102</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -263,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -294,6 +356,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -629,14 +692,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X13" sqref="X13"/>
+      <selection pane="bottomRight" activeCell="V23" sqref="V23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1809,8 +1872,66 @@
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
     </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="11">
+        <v>42138</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M16" s="11">
+        <v>42138</v>
+      </c>
+      <c r="W16" s="12">
+        <v>0.5083333333333333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F17" s="11">
+        <v>42152</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M17" s="11">
+        <v>42152</v>
+      </c>
+      <c r="W17" s="12">
+        <v>0.51874999999999993</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F18" s="11">
+        <v>42165</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I18" t="s">
+        <v>47</v>
+      </c>
+      <c r="M18" s="11">
+        <v>42165</v>
+      </c>
+      <c r="W18" s="12">
+        <v>0.55208333333333337</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>